<commit_message>
Update scripts to create Manual and Smoke testing issues
Manual tests issue_template has had Mantidplot and Vates removed, Sliceviewer added.
ISIS related manual tests were split out to issue_template_ISIS_11_2020.xlsx

SmokeTesting issue_template has had some minor updates, mostly related to plotting
create_issues_OS.py has separated the Smoke testing issues by OS

READMEs have been updates to reflect these changes AND the move to Personal Access Tokens
https://docs.github.com/en/github/authenticating-to-github/creating-a-personal-access-token
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwj28333\Documents\GitHub\SmokeTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Title</t>
   </si>
@@ -33,22 +33,84 @@
     <t>Assignee</t>
   </si>
   <si>
+    <t>Clean/Dirty Install Smoke Tests</t>
+  </si>
+  <si>
+    <t>Fitting Smoke Tests</t>
+  </si>
+  <si>
+    <t>Interface Smoke Tests</t>
+  </si>
+  <si>
+    <t>Plotting Smoke Tests</t>
+  </si>
+  <si>
+    <t>Python Smoke Tests</t>
+  </si>
+  <si>
+    <t>Emoji</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> :soap: :hankey:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> :muscle: :runner:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> :facepalm:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> :chart_with_upwards_trend: :bar_chart:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> :snake:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workspace/Algorithm Smoke Tests </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> :man_astronaut: :woman_astronaut: :space_invader:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Fitting to data [directions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/fitting_data/01_fitting_models_to_data.html#fitting-models-to-data)
+- [ ] Simple fit 
+- [ ] Activating the fitting tools 
+- [ ] Selecting the fitting range 
+- [ ] Other Fit Function Settings properties 
+- [ ] Setting up a fit model 
+- [ ] Adjusting fit function parameter 
+- [ ] Saving a model 
+- [ ] Tying and constraining fit parameters 
+- [ ] Execute your fit 
+- [ ] Inspecting a fit result 
+* Additional options [directions](https://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/fitting_data/03_fit_model_choices.html)
+- [ ] Non peak model + background 
+- [ ] User defined function </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Test that the Python scripting window works, [directions here](https://docs.mantidproject.org/nightly/workbench/scriptwindow.html)
+ - [ ] Editor options 
+ - [ ] Execution options 
+ - [ ] Script output  
+- [ ] Perform some workspace algebra 
+- [ ] Test numpy functionality 
+- [ ] Use the scripting window to run some scripts 
+- [ ] Run through some examples from [the documentation](http://www.mantidproject.org/Python_In_Mantid), 3 or 4 examples is enough </t>
+  </si>
+  <si>
     <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
-* Show detectors, check detector view GUI, follow non-Python directions [in the documentation](https://www.mantidproject.org/MantidPlot:_Instrument_View)
+* Show detectors, check Instrument Viewer, follow  directions [in the documentation](https://www.mantidproject.org/MantidPlot:_Instrument_View)
   - [ ] Render tab 
   - [ ] Draw tab 
   - [ ] Pick tab 
   - [ ] Instrument tree tab 
-* Test 5 - 10 random algorithms, follow [the documentation](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/algorithms_workspaces_and_histories/02_algorithms.html#algorithms)
+* Test 5 - 10 random algorithms, follow [the documentation](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/algorithms_workspaces_and_histories/02_algorithms.html#algorithms) and [pick your favourite](https://docs.mantidproject.org/v3.9.0/algorithms/)
  - [ ] Help button 
  - [ ] Validation of inputs 
  - [ ] Overwriting workspace 
  - [ ] Run the algorithm 
 - [ ] Check right-click options of the workspaces, they are listed [in the documentation](https://www.mantidproject.org/MantidPlot:_The_Workspace_Menu#Save_Nexus).
 </t>
-  </si>
-  <si>
-    <t>Workspace/Algorithm Smoke Tests</t>
   </si>
   <si>
     <t xml:space="preserve">### Dirty install
@@ -66,11 +128,11 @@
  * Clean out the registry
   * Load regedit (Command Prompt &gt; regedit)
   * Find `HKEY_CURRENT_USER &gt; SOFTWARE &gt; Mantid` delete it
-* OSX:
+**On macOS** :
  * Remove the application
  * Remove the `~/.mantid directory`
  * Remove `~/Library/Preferences/org.mantidproject.MantidPlot.plist`
-* Linux
+**On Linux** :
  * Remove the package: `/opt/Mantid`
  * Remove `~/.config/Mantid`
  * Remove `~/.mantid/`
@@ -79,74 +141,33 @@
 </t>
   </si>
   <si>
-    <t>Clean/Dirty Install Smoke Tests</t>
-  </si>
-  <si>
-    <t>Fitting Smoke Tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Fitting to data [directions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/fitting_data/01_fitting_models_to_data.html#fitting-models-to-data)
-- [ ] Simple fit 
-- [ ] Activating the fitting tools 
-- [ ] Selecting the fitting range 
-- [ ] Other Fit Function Settings properties 
-- [ ] Setting up a fit model 
-- [ ] Adjusting fit function parameter 
-- [ ] Saving a model 
-- [ ] Tying and constraining fit parameters 
-- [ ] Execute your fit 
-- [ ] Inspecting a fit result 
-* Additional options [directions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/fitting_data/02_fit_model_choices.html#fit-model-choices)
-- [ ] Non peak model + background 
-- [ ] User defined function </t>
-  </si>
-  <si>
-    <t>Interface Smoke Tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+    <t>## ISIS only, if possible, so catalogue access can be tested
 - [ ] Mantid opens without errors or warnings 
 - [ ] Every option in `Interface` opens a GUI 
 - [ ] Load some test data 
-- [ ] Catalogue opens  [directions here](https://www.mantidproject.org/Catalog_Search) 
-- [ ] Saving/loading projects works  [directions here](https://www.mantidproject.org/MantidPlot:_The_File_Menu#File-.3E_Save_Project_as...) </t>
-  </si>
-  <si>
-    <t>Plotting Smoke Tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* 1D plotting:[instructions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/loading_and_displaying_data/03_displaying_1D_data.html#displaying-1d-data)
+- [ ] Access Catalogue through algorithms (use Facilities account, same as for IDAaaS): [CatalogLogin](https://docs.mantidproject.org/v3.9.0/algorithms/CatalogLogin-v1.html) and [CatalogGetDataFiles](https://docs.mantidproject.org/v3.9.0/algorithms/CatalogGetDataFiles-v1.html)
+- [ ] Saving/loading projects works  [directions here](https://www.mantidproject.org/MantidPlot:_The_File_Menu#File-.3E_Save_Project_as...) 
+ - [ ] Alter preferences in [File &gt; Settings](https://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/useful/01_save_settings.html#settings) and check they are obeyed</t>
+  </si>
+  <si>
+    <t>* 1D plotting:[instructions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/loading_and_displaying_data/03_displaying_1D_data.html#displaying-1d-data)
  - [ ] Simple plot 
  - [ ] Another way to plot 
  - [ ] Adding curves to existing plots 
+ - [ ] Also, test out [waterfall](https://docs.mantidproject.org/nightly/plotting/WaterfallPlotsHelp.html#waterfall-plots) and [tiled]( https://docs.mantidproject.org/nightly/plotting/1DPlotsHelp.html#tiled-plots)
+ - [ ] Check Toolbar buttons
 * 2D plotting: [instructions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/loading_and_displaying_data/04_displaying_2D_data.html#displaying-2d-data)
  - [ ] Plot all spectra 
- - [ ] Plot from matrix 
  - [ ] Change colour map 
- - [ ] Contour plot 
- - [ ] Spectrum viewer 
-* 3D plotting:
+ - [ ] [Contour plot](https://docs.mantidproject.org/nightly/plotting/ColorfillPlotsHelp.html#contour-plots) (under 3D menu) 
+ - [ ] Check Toolbar buttons
+* [3D plotting](https://docs.mantidproject.org/nightly/plotting/3DPlotsHelp.html):
  - Load some data eg `LOQ7041` from the ISIS sample data
- - Double click the workspace to open the table view
- - Select the table
- - [ ] 3D plot becomes available as an option in the toolbar 
- - [ ] 3D wire frame 
- - [ ] 3D hidden line 
- - [ ] 3D polygon 
- - [ ] 3D wire surface </t>
-  </si>
-  <si>
-    <t>Python Smoke Tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Test that the Python scripting window works, [directions here](http://docs.mantidproject.org/v3.7.2/interfaces/ScriptingWindow.html)
- - [ ] Editor options 
- - [ ] Execution options 
- - [ ] Script output  
-- [ ] Perform some workspace algebra 
-- [ ] Test numpy functionality 
-- [ ] Use the scripting window to run some scripts 
-- [ ] Run through some examples from [the documentation](http://www.mantidproject.org/Python_In_Mantid), 3 or 4 examples is enough </t>
+ - [ ] 3D surface
+ - [ ] 3D wire frame  
+ - [ ] Check Toolbar buttons
+ ## Sliceviewer
+ - [ ] Overly long instructions (don't spend hours!) and data [here](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html). In particular try editing the data in a workspace while it is open in Sliceviewer! ([step 10](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html#alter-the-underlying-workspace))</t>
   </si>
 </sst>
 </file>
@@ -1022,168 +1043,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="46" style="1" customWidth="1"/>
+    <col min="3" max="3" width="72.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2"/>
+    </row>
+    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2"/>
-    </row>
-    <row r="3" spans="1:3" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3"/>
-    </row>
-    <row r="4" spans="1:3" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4"/>
-    </row>
-    <row r="5" spans="1:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5"/>
-    </row>
-    <row r="6" spans="1:3" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="1:3" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7"/>
-    </row>
-    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="C8"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15"/>
-    </row>
-    <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28"/>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29"/>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30"/>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C31"/>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C32"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33"/>
+      <c r="B8" s="4"/>
+      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F7"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C33">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G7"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D33">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1196,7 +1239,7 @@
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C34:C40</xm:sqref>
+          <xm:sqref>D34:D40</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Update smoke testing files.
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-development\mantid-docs\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="34545" yWindow="-12855" windowWidth="31665" windowHeight="16500"/>
   </bookViews>
   <sheets>
-    <sheet name="issues" sheetId="1" r:id="rId1"/>
+    <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
+    <sheet name="issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Title</t>
   </si>
@@ -168,6 +169,34 @@
  - [ ] Check Toolbar buttons
  ## Sliceviewer
  - [ ] Overly long instructions (don't spend hours!) and data [here](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html). In particular try editing the data in a workspace while it is open in Sliceviewer! ([step 10](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html#alter-the-underlying-workspace))</t>
+  </si>
+  <si>
+    <t>Operating System</t>
+  </si>
+  <si>
+    <t>Additional Instructions</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>MacOS</t>
+  </si>
+  <si>
+    <t>Redhat</t>
+  </si>
+  <si>
+    <t>Ubuntu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>## If at ISIS, please test on IDAaaS
+* Follow the instructions [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK) to test Mantid on IDAaaS</t>
+  </si>
+  <si>
+    <t>* Follow the instructions [here](https://download.mantidproject.org/ubuntu.html) to install the .deb for Ubuntu</t>
   </si>
 </sst>
 </file>
@@ -670,7 +699,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -682,6 +711,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1043,10 +1076,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove outdated instruction for clean/dirty install.
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34545" yWindow="-12855" windowWidth="31665" windowHeight="16500"/>
+    <workbookView xWindow="34545" yWindow="-12855" windowWidth="31665" windowHeight="16500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -111,34 +111,6 @@
  - [ ] Overwriting workspace 
  - [ ] Run the algorithm 
 - [ ] Check right-click options of the workspaces, they are listed [in the documentation](https://www.mantidproject.org/MantidPlot:_The_Workspace_Menu#Save_Nexus).
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">### Dirty install
-* Make sure that you have several versions of Mantid installed
- * Last release
- * A nightly
- * If possible an old release
-* Install the latest version of the new Mantid
-- [ ] Check that Mantid boots up correctly
-### Clean install
-* Remove all existing Mantid versions and associated files
-* Windows:
- * Uninstall the program
- * Clear shortcuts from desktop
- * Clean out the registry
-  * Load regedit (Command Prompt &gt; regedit)
-  * Find `HKEY_CURRENT_USER &gt; SOFTWARE &gt; Mantid` delete it
-**On macOS** :
- * Remove the application
- * Remove the `~/.mantid directory`
- * Remove `~/Library/Preferences/org.mantidproject.MantidPlot.plist`
-**On Linux** :
- * Remove the package: `/opt/Mantid`
- * Remove `~/.config/Mantid`
- * Remove `~/.mantid/`
-* Re-install the latest version of the new Mantid
-- [ ] Check that Mantid boots up correctly
 </t>
   </si>
   <si>
@@ -197,6 +169,33 @@
   </si>
   <si>
     <t>* Follow the instructions [here](https://download.mantidproject.org/ubuntu.html) to install the .deb for Ubuntu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">### Dirty install
+* Make sure that you have several versions of Mantid installed
+ * Last release
+ * A nightly
+ * If possible an old release
+* Install the latest version of the new Mantid
+- [ ] Check that Mantid boots up correctly
+### Clean install
+* Remove all existing Mantid versions and associated files
+* Windows:
+ * Uninstall the program
+ * Clear shortcuts from desktop
+ * Clean out the registry
+  * Load regedit (Command Prompt &gt; regedit)
+**On macOS** :
+ * Remove the application
+ * Remove the `~/.mantid directory`
+ * Remove `~/Library/Preferences/org.mantidproject.MantidPlot.plist`
+**On Linux** :
+ * Remove the package: `/opt/Mantid`
+ * Remove `~/.config/Mantid`
+ * Remove `~/.mantid/`
+* Re-install the latest version of the new Mantid
+- [ ] Check that Mantid boots up correctly
+</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1090,42 +1089,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1138,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1171,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D2"/>
     </row>
@@ -1196,7 +1195,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4"/>
     </row>
@@ -1208,7 +1207,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5"/>
     </row>

</xml_diff>

<commit_message>
Update Smoke testing spreadsheet
Update InstrumentViewer links
Update Catalog Links
Correct OS specific instructions for clean install
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-development\mantid-docs\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/SmokeTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B3F720-54D6-194A-AC64-3B21D8D5EF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34545" yWindow="-12855" windowWidth="31665" windowHeight="16500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21600" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -97,30 +98,6 @@
 - [ ] Test numpy functionality 
 - [ ] Use the scripting window to run some scripts 
 - [ ] Run through some examples from [the documentation](http://www.mantidproject.org/Python_In_Mantid), 3 or 4 examples is enough </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
-* Show detectors, check Instrument Viewer, follow  directions [in the documentation](https://www.mantidproject.org/MantidPlot:_Instrument_View)
-  - [ ] Render tab 
-  - [ ] Draw tab 
-  - [ ] Pick tab 
-  - [ ] Instrument tree tab 
-* Test 5 - 10 random algorithms, follow [the documentation](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/algorithms_workspaces_and_histories/02_algorithms.html#algorithms) and [pick your favourite](https://docs.mantidproject.org/v3.9.0/algorithms/)
- - [ ] Help button 
- - [ ] Validation of inputs 
- - [ ] Overwriting workspace 
- - [ ] Run the algorithm 
-- [ ] Check right-click options of the workspaces, they are listed [in the documentation](https://www.mantidproject.org/MantidPlot:_The_Workspace_Menu#Save_Nexus).
-</t>
-  </si>
-  <si>
-    <t>## ISIS only, if possible, so catalogue access can be tested
-- [ ] Mantid opens without errors or warnings 
-- [ ] Every option in `Interface` opens a GUI 
-- [ ] Load some test data 
-- [ ] Access Catalogue through algorithms (use Facilities account, same as for IDAaaS): [CatalogLogin](https://docs.mantidproject.org/v3.9.0/algorithms/CatalogLogin-v1.html) and [CatalogGetDataFiles](https://docs.mantidproject.org/v3.9.0/algorithms/CatalogGetDataFiles-v1.html)
-- [ ] Saving/loading projects works  [directions here](https://www.mantidproject.org/MantidPlot:_The_File_Menu#File-.3E_Save_Project_as...) 
- - [ ] Alter preferences in [File &gt; Settings](https://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/useful/01_save_settings.html#settings) and check they are obeyed</t>
   </si>
   <si>
     <t>* 1D plotting:[instructions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/loading_and_displaying_data/03_displaying_1D_data.html#displaying-1d-data)
@@ -180,28 +157,52 @@
 - [ ] Check that Mantid boots up correctly
 ### Clean install
 * Remove all existing Mantid versions and associated files
-* Windows:
+**On Windows**:
  * Uninstall the program
  * Clear shortcuts from desktop
- * Clean out the registry
-  * Load regedit (Command Prompt &gt; regedit)
+  * Remove the mantid  files in %APPDATA%
 **On macOS** :
  * Remove the application
  * Remove the `~/.mantid directory`
- * Remove `~/Library/Preferences/org.mantidproject.MantidPlot.plist`
+ * Remove (or rename) `~/Library/Preferences/org.python.python.Python.plist`  and `~/Library/Preferences/org.python.python.plist` 
 **On Linux** :
  * Remove the package: `/opt/Mantid`
  * Remove `~/.config/Mantid`
  * Remove `~/.mantid/`
-* Re-install the latest version of the new Mantid
+Re-install the latest version of the new Mantid
 - [ ] Check that Mantid boots up correctly
+</t>
+  </si>
+  <si>
+    <t>## ISIS only, if possible, so catalogue access can be tested
+- [ ] Mantid opens without errors or warnings 
+- [ ] Every option in `Interface` opens a GUI 
+- [ ] Load some test data 
+- [ ] Access Catalogue through algorithms (use Facilities account, same as for IDAaaS): [CatalogLogin](https://docs.mantidproject.org/algorithms/CatalogLogin-v1.html) and [CatalogGetDataFiles](https://docs.mantidproject.org/algorithms/CatalogGetDataFiles-v1.html)
+- [ ] Saving/loading projects works  [directions here](https://www.mantidproject.org/MantidPlot:_The_File_Menu#File-.3E_Save_Project_as...) 
+ - [ ] Alter preferences in [File &gt; Settings](https://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/useful/01_save_settings.html#settings) and check they are obeyed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
+* Show detectors on these workspaces
+* Check Instrument Viewer for these workspaces, follow  documentation for  [Instrument Viewer Widget](https://docs.mantidproject.org/workbench/instrumentviewer.html) and some more detail on the picking tools in the [Basic Course](https://docs.mantidproject.org/tutorials/mantid_basic_course/connecting_data_to_instruments/03_investigating_data.html)
+  - [ ] Render tab 
+  - [ ] Draw tab 
+  - [ ] Pick tab 
+  - [ ] Instrument tree tab 
+* Test 5 - 10 random algorithms, follow [how to run Algorithms](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/algorithms_workspaces_and_histories/02_algorithms.html#algorithms) and [pick your favourite](https://docs.mantidproject.org/algorithms/)
+ - [ ] Help button 
+ - [ ] Validation of inputs 
+ - [ ] Overwriting workspace 
+ - [ ] Run the algorithm 
+- [ ] Check right-click options of the workspaces, they are listed [in the documentation](https://www.mantidproject.org/MantidPlot:_The_Workspace_Menu#Save_Nexus).
 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -864,6 +865,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -899,6 +917,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1074,57 +1109,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" customWidth="1"/>
+    <col min="2" max="2" width="64.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1134,22 +1169,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="46" style="1" customWidth="1"/>
-    <col min="3" max="3" width="72.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="72.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1163,7 +1198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1171,11 +1206,11 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1187,7 +1222,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1195,11 +1230,11 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1207,11 +1242,11 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1223,7 +1258,7 @@
       </c>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1231,94 +1266,94 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D16"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D18"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D19"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D21"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D22"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D23"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D24"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D25"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D26"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D27"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D28"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D29"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D30"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D31"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D32"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G7"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D33">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G7" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D33" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1327,7 +1362,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Add Conda test issue to SmokeTests
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/SmokeTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B3F720-54D6-194A-AC64-3B21D8D5EF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BDF3F2-F789-414D-ACF7-7F4AC2156AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21600" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49220" yWindow="500" windowWidth="22780" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Title</t>
   </si>
@@ -90,14 +90,83 @@
 - [ ] User defined function </t>
   </si>
   <si>
-    <t xml:space="preserve">* Test that the Python scripting window works, [directions here](https://docs.mantidproject.org/nightly/workbench/scriptwindow.html)
- - [ ] Editor options 
- - [ ] Execution options 
- - [ ] Script output  
-- [ ] Perform some workspace algebra 
-- [ ] Test numpy functionality 
-- [ ] Use the scripting window to run some scripts 
-- [ ] Run through some examples from [the documentation](http://www.mantidproject.org/Python_In_Mantid), 3 or 4 examples is enough </t>
+    <t>Operating System</t>
+  </si>
+  <si>
+    <t>Additional Instructions</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>MacOS</t>
+  </si>
+  <si>
+    <t>Redhat</t>
+  </si>
+  <si>
+    <t>Ubuntu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>## If at ISIS, please test on IDAaaS
+* Follow the instructions [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK) to test Mantid on IDAaaS</t>
+  </si>
+  <si>
+    <t>* Follow the instructions [here](https://download.mantidproject.org/ubuntu.html) to install the .deb for Ubuntu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
+* Show detectors on these workspaces
+* Check Instrument Viewer for these workspaces, follow  documentation for  [Instrument Viewer Widget](https://docs.mantidproject.org/workbench/instrumentviewer.html) and some more detail on the picking tools in the [Basic Course](https://docs.mantidproject.org/tutorials/mantid_basic_course/connecting_data_to_instruments/03_investigating_data.html)
+  - [ ] Render tab 
+  - [ ] Draw tab 
+  - [ ] Pick tab 
+  - [ ] Instrument tree tab 
+* Test 5 - 10 random algorithms, follow [how to run Algorithms](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/algorithms_workspaces_and_histories/02_algorithms.html#algorithms) and [pick your favourite](https://docs.mantidproject.org/algorithms/)
+ - [ ] Help button 
+ - [ ] Validation of inputs 
+ - [ ] Overwriting workspace 
+ - [ ] Run the algorithm 
+- [ ] Check right-click options of the workspaces, they are listed [in the documentation](https://www.mantidproject.org/MantidPlot:_The_Workspace_Menu#Save_Nexus).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">### Dirty install
+* Make sure that you have several versions of Mantid installed
+ * Last release
+ * A nightly
+ * If possible an old release
+* Install the new release candidate of Mantid
+- [ ] Check that Mantid boots up correctly
+### Clean install
+* Remove all existing Mantid versions and associated files
+**On Windows**:
+ * Uninstall the program
+ * Clear shortcuts from desktop
+ * Remove the mantid  files in %APPDATA%
+**On macOS** :
+ * Remove the application
+ * Remove the `~/.mantid directory`
+ * Remove (or rename) `~/Library/Preferences/org.python.python.Python.plist`  and `~/Library/Preferences/org.python.python.plist` 
+**On Linux** :
+ * Remove the package: `/opt/Mantid`
+ * Remove `~/.config/Mantid`
+ * Remove `~/.mantid/`
+Re-install the new release candidate of Mantid
+- [ ] Check that Mantid boots up correctly
+</t>
+  </si>
+  <si>
+    <t>## ISIS only, if possible, so catalogue access can be tested
+- [ ] MantidWorkbench opens without errors or warnings 
+- [ ] Every option in `Interface` opens a GUI 
+- [ ] Load some test data 
+- [ ] Access Catalogue through algorithms (use Facilities account, same as for IDAaaS): [CatalogLogin](https://docs.mantidproject.org/algorithms/CatalogLogin-v1.html) and [CatalogGetDataFiles](https://docs.mantidproject.org/algorithms/CatalogGetDataFiles-v1.html)
+- [ ] Saving/loading projects works 
+ - [ ] Alter preferences in [File &gt; Settings](https://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/useful/01_save_settings.html#settings) and check they are obeyed</t>
   </si>
   <si>
     <t>* 1D plotting:[instructions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/loading_and_displaying_data/03_displaying_1D_data.html#displaying-1d-data)
@@ -117,86 +186,23 @@
  - [ ] 3D wire frame  
  - [ ] Check Toolbar buttons
  ## Sliceviewer
- - [ ] Overly long instructions (don't spend hours!) and data [here](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html). In particular try editing the data in a workspace while it is open in Sliceviewer! ([step 10](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html#alter-the-underlying-workspace))</t>
-  </si>
-  <si>
-    <t>Operating System</t>
-  </si>
-  <si>
-    <t>Additional Instructions</t>
-  </si>
-  <si>
-    <t>Windows</t>
-  </si>
-  <si>
-    <t>MacOS</t>
-  </si>
-  <si>
-    <t>Redhat</t>
-  </si>
-  <si>
-    <t>Ubuntu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>## If at ISIS, please test on IDAaaS
-* Follow the instructions [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK) to test Mantid on IDAaaS</t>
-  </si>
-  <si>
-    <t>* Follow the instructions [here](https://download.mantidproject.org/ubuntu.html) to install the .deb for Ubuntu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">### Dirty install
-* Make sure that you have several versions of Mantid installed
- * Last release
- * A nightly
- * If possible an old release
-* Install the latest version of the new Mantid
-- [ ] Check that Mantid boots up correctly
-### Clean install
-* Remove all existing Mantid versions and associated files
-**On Windows**:
- * Uninstall the program
- * Clear shortcuts from desktop
-  * Remove the mantid  files in %APPDATA%
-**On macOS** :
- * Remove the application
- * Remove the `~/.mantid directory`
- * Remove (or rename) `~/Library/Preferences/org.python.python.Python.plist`  and `~/Library/Preferences/org.python.python.plist` 
-**On Linux** :
- * Remove the package: `/opt/Mantid`
- * Remove `~/.config/Mantid`
- * Remove `~/.mantid/`
-Re-install the latest version of the new Mantid
-- [ ] Check that Mantid boots up correctly
-</t>
-  </si>
-  <si>
-    <t>## ISIS only, if possible, so catalogue access can be tested
-- [ ] Mantid opens without errors or warnings 
-- [ ] Every option in `Interface` opens a GUI 
-- [ ] Load some test data 
-- [ ] Access Catalogue through algorithms (use Facilities account, same as for IDAaaS): [CatalogLogin](https://docs.mantidproject.org/algorithms/CatalogLogin-v1.html) and [CatalogGetDataFiles](https://docs.mantidproject.org/algorithms/CatalogGetDataFiles-v1.html)
-- [ ] Saving/loading projects works  [directions here](https://www.mantidproject.org/MantidPlot:_The_File_Menu#File-.3E_Save_Project_as...) 
- - [ ] Alter preferences in [File &gt; Settings](https://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/useful/01_save_settings.html#settings) and check they are obeyed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
-* Show detectors on these workspaces
-* Check Instrument Viewer for these workspaces, follow  documentation for  [Instrument Viewer Widget](https://docs.mantidproject.org/workbench/instrumentviewer.html) and some more detail on the picking tools in the [Basic Course](https://docs.mantidproject.org/tutorials/mantid_basic_course/connecting_data_to_instruments/03_investigating_data.html)
-  - [ ] Render tab 
-  - [ ] Draw tab 
-  - [ ] Pick tab 
-  - [ ] Instrument tree tab 
-* Test 5 - 10 random algorithms, follow [how to run Algorithms](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/algorithms_workspaces_and_histories/02_algorithms.html#algorithms) and [pick your favourite](https://docs.mantidproject.org/algorithms/)
- - [ ] Help button 
- - [ ] Validation of inputs 
- - [ ] Overwriting workspace 
- - [ ] Run the algorithm 
-- [ ] Check right-click options of the workspaces, they are listed [in the documentation](https://www.mantidproject.org/MantidPlot:_The_Workspace_Menu#Save_Nexus).
-</t>
+ - [ ] Overly long instructions (don't spend  long!) and data [here](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html). In particular try editing the data in a workspace while it is open in Sliceviewer!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Test that the Python scripting window works, [directions here](https://docs.mantidproject.org/nightly/workbench/scriptwindow.html)
+ - [ ] Editor options 
+ - [ ] Execution options 
+ - [ ] Script output  
+- [ ] Perform some workspace algebra 
+- [ ] Test numpy functionality 
+- [ ] Use the scripting window to run some scripts 
+- [ ] Run through some examples from [the documentation](https://docs.mantidproject.org/nightly/tutorials/python_in_mantid/index.html), 3 or 4 examples from the Solutions is enough </t>
+  </si>
+  <si>
+    <t>Conda Package Tests</t>
+  </si>
+  <si>
+    <t>Quickly run through some of the other Smoke testing instructions on the separate Conda release package. The most useful tests is to check many different dependencies, such as numpy and matpltlib in the editor, and opening the interfaces.</t>
   </si>
 </sst>
 </file>
@@ -1124,42 +1130,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1173,7 +1179,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1206,7 +1212,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2"/>
     </row>
@@ -1230,7 +1236,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4"/>
     </row>
@@ -1242,7 +1248,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D5"/>
     </row>
@@ -1254,7 +1260,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D6"/>
     </row>
@@ -1266,13 +1272,20 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add Conda test issue to SmokeTests (#103)
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/SmokeTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B3F720-54D6-194A-AC64-3B21D8D5EF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BDF3F2-F789-414D-ACF7-7F4AC2156AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21600" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49220" yWindow="500" windowWidth="22780" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Title</t>
   </si>
@@ -90,14 +90,83 @@
 - [ ] User defined function </t>
   </si>
   <si>
-    <t xml:space="preserve">* Test that the Python scripting window works, [directions here](https://docs.mantidproject.org/nightly/workbench/scriptwindow.html)
- - [ ] Editor options 
- - [ ] Execution options 
- - [ ] Script output  
-- [ ] Perform some workspace algebra 
-- [ ] Test numpy functionality 
-- [ ] Use the scripting window to run some scripts 
-- [ ] Run through some examples from [the documentation](http://www.mantidproject.org/Python_In_Mantid), 3 or 4 examples is enough </t>
+    <t>Operating System</t>
+  </si>
+  <si>
+    <t>Additional Instructions</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>MacOS</t>
+  </si>
+  <si>
+    <t>Redhat</t>
+  </si>
+  <si>
+    <t>Ubuntu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>## If at ISIS, please test on IDAaaS
+* Follow the instructions [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK) to test Mantid on IDAaaS</t>
+  </si>
+  <si>
+    <t>* Follow the instructions [here](https://download.mantidproject.org/ubuntu.html) to install the .deb for Ubuntu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
+* Show detectors on these workspaces
+* Check Instrument Viewer for these workspaces, follow  documentation for  [Instrument Viewer Widget](https://docs.mantidproject.org/workbench/instrumentviewer.html) and some more detail on the picking tools in the [Basic Course](https://docs.mantidproject.org/tutorials/mantid_basic_course/connecting_data_to_instruments/03_investigating_data.html)
+  - [ ] Render tab 
+  - [ ] Draw tab 
+  - [ ] Pick tab 
+  - [ ] Instrument tree tab 
+* Test 5 - 10 random algorithms, follow [how to run Algorithms](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/algorithms_workspaces_and_histories/02_algorithms.html#algorithms) and [pick your favourite](https://docs.mantidproject.org/algorithms/)
+ - [ ] Help button 
+ - [ ] Validation of inputs 
+ - [ ] Overwriting workspace 
+ - [ ] Run the algorithm 
+- [ ] Check right-click options of the workspaces, they are listed [in the documentation](https://www.mantidproject.org/MantidPlot:_The_Workspace_Menu#Save_Nexus).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">### Dirty install
+* Make sure that you have several versions of Mantid installed
+ * Last release
+ * A nightly
+ * If possible an old release
+* Install the new release candidate of Mantid
+- [ ] Check that Mantid boots up correctly
+### Clean install
+* Remove all existing Mantid versions and associated files
+**On Windows**:
+ * Uninstall the program
+ * Clear shortcuts from desktop
+ * Remove the mantid  files in %APPDATA%
+**On macOS** :
+ * Remove the application
+ * Remove the `~/.mantid directory`
+ * Remove (or rename) `~/Library/Preferences/org.python.python.Python.plist`  and `~/Library/Preferences/org.python.python.plist` 
+**On Linux** :
+ * Remove the package: `/opt/Mantid`
+ * Remove `~/.config/Mantid`
+ * Remove `~/.mantid/`
+Re-install the new release candidate of Mantid
+- [ ] Check that Mantid boots up correctly
+</t>
+  </si>
+  <si>
+    <t>## ISIS only, if possible, so catalogue access can be tested
+- [ ] MantidWorkbench opens without errors or warnings 
+- [ ] Every option in `Interface` opens a GUI 
+- [ ] Load some test data 
+- [ ] Access Catalogue through algorithms (use Facilities account, same as for IDAaaS): [CatalogLogin](https://docs.mantidproject.org/algorithms/CatalogLogin-v1.html) and [CatalogGetDataFiles](https://docs.mantidproject.org/algorithms/CatalogGetDataFiles-v1.html)
+- [ ] Saving/loading projects works 
+ - [ ] Alter preferences in [File &gt; Settings](https://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/useful/01_save_settings.html#settings) and check they are obeyed</t>
   </si>
   <si>
     <t>* 1D plotting:[instructions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/loading_and_displaying_data/03_displaying_1D_data.html#displaying-1d-data)
@@ -117,86 +186,23 @@
  - [ ] 3D wire frame  
  - [ ] Check Toolbar buttons
  ## Sliceviewer
- - [ ] Overly long instructions (don't spend hours!) and data [here](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html). In particular try editing the data in a workspace while it is open in Sliceviewer! ([step 10](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html#alter-the-underlying-workspace))</t>
-  </si>
-  <si>
-    <t>Operating System</t>
-  </si>
-  <si>
-    <t>Additional Instructions</t>
-  </si>
-  <si>
-    <t>Windows</t>
-  </si>
-  <si>
-    <t>MacOS</t>
-  </si>
-  <si>
-    <t>Redhat</t>
-  </si>
-  <si>
-    <t>Ubuntu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>## If at ISIS, please test on IDAaaS
-* Follow the instructions [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK) to test Mantid on IDAaaS</t>
-  </si>
-  <si>
-    <t>* Follow the instructions [here](https://download.mantidproject.org/ubuntu.html) to install the .deb for Ubuntu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">### Dirty install
-* Make sure that you have several versions of Mantid installed
- * Last release
- * A nightly
- * If possible an old release
-* Install the latest version of the new Mantid
-- [ ] Check that Mantid boots up correctly
-### Clean install
-* Remove all existing Mantid versions and associated files
-**On Windows**:
- * Uninstall the program
- * Clear shortcuts from desktop
-  * Remove the mantid  files in %APPDATA%
-**On macOS** :
- * Remove the application
- * Remove the `~/.mantid directory`
- * Remove (or rename) `~/Library/Preferences/org.python.python.Python.plist`  and `~/Library/Preferences/org.python.python.plist` 
-**On Linux** :
- * Remove the package: `/opt/Mantid`
- * Remove `~/.config/Mantid`
- * Remove `~/.mantid/`
-Re-install the latest version of the new Mantid
-- [ ] Check that Mantid boots up correctly
-</t>
-  </si>
-  <si>
-    <t>## ISIS only, if possible, so catalogue access can be tested
-- [ ] Mantid opens without errors or warnings 
-- [ ] Every option in `Interface` opens a GUI 
-- [ ] Load some test data 
-- [ ] Access Catalogue through algorithms (use Facilities account, same as for IDAaaS): [CatalogLogin](https://docs.mantidproject.org/algorithms/CatalogLogin-v1.html) and [CatalogGetDataFiles](https://docs.mantidproject.org/algorithms/CatalogGetDataFiles-v1.html)
-- [ ] Saving/loading projects works  [directions here](https://www.mantidproject.org/MantidPlot:_The_File_Menu#File-.3E_Save_Project_as...) 
- - [ ] Alter preferences in [File &gt; Settings](https://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/useful/01_save_settings.html#settings) and check they are obeyed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
-* Show detectors on these workspaces
-* Check Instrument Viewer for these workspaces, follow  documentation for  [Instrument Viewer Widget](https://docs.mantidproject.org/workbench/instrumentviewer.html) and some more detail on the picking tools in the [Basic Course](https://docs.mantidproject.org/tutorials/mantid_basic_course/connecting_data_to_instruments/03_investigating_data.html)
-  - [ ] Render tab 
-  - [ ] Draw tab 
-  - [ ] Pick tab 
-  - [ ] Instrument tree tab 
-* Test 5 - 10 random algorithms, follow [how to run Algorithms](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/algorithms_workspaces_and_histories/02_algorithms.html#algorithms) and [pick your favourite](https://docs.mantidproject.org/algorithms/)
- - [ ] Help button 
- - [ ] Validation of inputs 
- - [ ] Overwriting workspace 
- - [ ] Run the algorithm 
-- [ ] Check right-click options of the workspaces, they are listed [in the documentation](https://www.mantidproject.org/MantidPlot:_The_Workspace_Menu#Save_Nexus).
-</t>
+ - [ ] Overly long instructions (don't spend  long!) and data [here](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html). In particular try editing the data in a workspace while it is open in Sliceviewer!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Test that the Python scripting window works, [directions here](https://docs.mantidproject.org/nightly/workbench/scriptwindow.html)
+ - [ ] Editor options 
+ - [ ] Execution options 
+ - [ ] Script output  
+- [ ] Perform some workspace algebra 
+- [ ] Test numpy functionality 
+- [ ] Use the scripting window to run some scripts 
+- [ ] Run through some examples from [the documentation](https://docs.mantidproject.org/nightly/tutorials/python_in_mantid/index.html), 3 or 4 examples from the Solutions is enough </t>
+  </si>
+  <si>
+    <t>Conda Package Tests</t>
+  </si>
+  <si>
+    <t>Quickly run through some of the other Smoke testing instructions on the separate Conda release package. The most useful tests is to check many different dependencies, such as numpy and matpltlib in the editor, and opening the interfaces.</t>
   </si>
 </sst>
 </file>
@@ -1124,42 +1130,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1173,7 +1179,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1206,7 +1212,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2"/>
     </row>
@@ -1230,7 +1236,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4"/>
     </row>
@@ -1242,7 +1248,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D5"/>
     </row>
@@ -1254,7 +1260,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D6"/>
     </row>
@@ -1266,13 +1272,20 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update SmokeTests to add conda and Personal Access Token
Add 2 second wait between POST requests to workaround GitHub API secondary rate limits
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/SmokeTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BDF3F2-F789-414D-ACF7-7F4AC2156AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494EEE5A-91A5-B449-BA8C-814C782B2AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49220" yWindow="500" windowWidth="22780" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49220" yWindow="500" windowWidth="22780" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Title</t>
   </si>
@@ -197,12 +197,6 @@
 - [ ] Test numpy functionality 
 - [ ] Use the scripting window to run some scripts 
 - [ ] Run through some examples from [the documentation](https://docs.mantidproject.org/nightly/tutorials/python_in_mantid/index.html), 3 or 4 examples from the Solutions is enough </t>
-  </si>
-  <si>
-    <t>Conda Package Tests</t>
-  </si>
-  <si>
-    <t>Quickly run through some of the other Smoke testing instructions on the separate Conda release package. The most useful tests is to check many different dependencies, such as numpy and matpltlib in the editor, and opening the interfaces.</t>
   </si>
 </sst>
 </file>
@@ -1116,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1128,15 +1122,18 @@
     <col min="2" max="2" width="64.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
@@ -1144,7 +1141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
@@ -1152,7 +1149,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -1160,7 +1157,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
@@ -1178,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1200,9 +1197,6 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1276,16 +1270,9 @@
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updates after release 6.5
Add conda instructions to OS Smoke test
update SANS manual testing link
add superplot to plot images powerpoint
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/SmokeTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494EEE5A-91A5-B449-BA8C-814C782B2AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAE0071-BAD2-D849-8194-06456E17F9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49220" yWindow="500" windowWidth="22780" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -106,16 +106,6 @@
   </si>
   <si>
     <t>Ubuntu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>## If at ISIS, please test on IDAaaS
-* Follow the instructions [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK) to test Mantid on IDAaaS</t>
-  </si>
-  <si>
-    <t>* Follow the instructions [here](https://download.mantidproject.org/ubuntu.html) to install the .deb for Ubuntu</t>
   </si>
   <si>
     <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
@@ -197,6 +187,28 @@
 - [ ] Test numpy functionality 
 - [ ] Use the scripting window to run some scripts 
 - [ ] Run through some examples from [the documentation](https://docs.mantidproject.org/nightly/tutorials/python_in_mantid/index.html), 3 or 4 examples from the Solutions is enough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* To install the tar.xz package for Linux, run `(sudo) tar -xJf mantid-VA.B.C.tar.xz` in a terminal and it will unzip the package in your current working directory. 
+* To install via conda:
+  - Use Intel Conda and make sure conda-forge is added to channels
+  - In terminal, create a new empty environment and activate it
+  - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.
+</t>
+  </si>
+  <si>
+    <t>## If at ISIS, please test on IDAaaS
+* Either install on a developer mantid IDAaaS instance with credentials [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK)
+* Or install via conda on a normal IDAaaS instance:
+  - In terminal, create a new empty environment and activate it
+  - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.</t>
+  </si>
+  <si>
+    <t>We must test the installer package and install direct from conda.
+* To install via conda:
+  - Use Intel Conda and make sure conda-forge is added to channels
+  - In terminal, create a new empty environment and activate it
+  - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1125,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1138,7 +1150,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
@@ -1146,7 +1158,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1154,7 +1166,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1162,7 +1174,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1218,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2"/>
     </row>
@@ -1230,7 +1242,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4"/>
     </row>
@@ -1242,7 +1254,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5"/>
     </row>
@@ -1254,7 +1266,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6"/>
     </row>
@@ -1266,7 +1278,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7"/>
     </row>

</xml_diff>

<commit_message>
Updates after release 6.5 (#106)
Add conda instructions to OS Smoke test
update SANS manual testing link
add superplot to plot images powerpoint
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/SmokeTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494EEE5A-91A5-B449-BA8C-814C782B2AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAE0071-BAD2-D849-8194-06456E17F9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49220" yWindow="500" windowWidth="22780" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -106,16 +106,6 @@
   </si>
   <si>
     <t>Ubuntu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>## If at ISIS, please test on IDAaaS
-* Follow the instructions [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK) to test Mantid on IDAaaS</t>
-  </si>
-  <si>
-    <t>* Follow the instructions [here](https://download.mantidproject.org/ubuntu.html) to install the .deb for Ubuntu</t>
   </si>
   <si>
     <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
@@ -197,6 +187,28 @@
 - [ ] Test numpy functionality 
 - [ ] Use the scripting window to run some scripts 
 - [ ] Run through some examples from [the documentation](https://docs.mantidproject.org/nightly/tutorials/python_in_mantid/index.html), 3 or 4 examples from the Solutions is enough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* To install the tar.xz package for Linux, run `(sudo) tar -xJf mantid-VA.B.C.tar.xz` in a terminal and it will unzip the package in your current working directory. 
+* To install via conda:
+  - Use Intel Conda and make sure conda-forge is added to channels
+  - In terminal, create a new empty environment and activate it
+  - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.
+</t>
+  </si>
+  <si>
+    <t>## If at ISIS, please test on IDAaaS
+* Either install on a developer mantid IDAaaS instance with credentials [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK)
+* Or install via conda on a normal IDAaaS instance:
+  - In terminal, create a new empty environment and activate it
+  - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.</t>
+  </si>
+  <si>
+    <t>We must test the installer package and install direct from conda.
+* To install via conda:
+  - Use Intel Conda and make sure conda-forge is added to channels
+  - In terminal, create a new empty environment and activate it
+  - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1125,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1138,7 +1150,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
@@ -1146,7 +1158,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1154,7 +1166,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1162,7 +1174,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1218,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2"/>
     </row>
@@ -1230,7 +1242,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4"/>
     </row>
@@ -1242,7 +1254,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5"/>
     </row>
@@ -1254,7 +1266,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6"/>
     </row>
@@ -1266,7 +1278,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7"/>
     </row>

</xml_diff>

<commit_message>
Merge Redhat and Ubuntu smoketesting
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/SmokeTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAE0071-BAD2-D849-8194-06456E17F9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955D629F-D42C-4942-9DFA-F56EDFB02A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Title</t>
   </si>
@@ -100,12 +100,6 @@
   </si>
   <si>
     <t>MacOS</t>
-  </si>
-  <si>
-    <t>Redhat</t>
-  </si>
-  <si>
-    <t>Ubuntu</t>
   </si>
   <si>
     <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
@@ -197,18 +191,14 @@
 </t>
   </si>
   <si>
-    <t>## If at ISIS, please test on IDAaaS
-* Either install on a developer mantid IDAaaS instance with credentials [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK)
-* Or install via conda on a normal IDAaaS instance:
-  - In terminal, create a new empty environment and activate it
-  - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.</t>
-  </si>
-  <si>
     <t>We must test the installer package and install direct from conda.
 * To install via conda:
   - Use Intel Conda and make sure conda-forge is added to channels
   - In terminal, create a new empty environment and activate it
   - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.</t>
+  </si>
+  <si>
+    <t>Linux</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1115,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1150,7 +1140,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
@@ -1158,24 +1148,20 @@
         <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>28</v>
-      </c>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1218,7 +1204,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2"/>
     </row>
@@ -1242,7 +1228,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4"/>
     </row>
@@ -1254,7 +1240,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5"/>
     </row>
@@ -1266,7 +1252,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6"/>
     </row>
@@ -1278,7 +1264,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7"/>
     </row>

</xml_diff>

<commit_message>
Merge Redhat and Ubuntu smoketesting (#107)
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/SmokeTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAE0071-BAD2-D849-8194-06456E17F9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955D629F-D42C-4942-9DFA-F56EDFB02A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Title</t>
   </si>
@@ -100,12 +100,6 @@
   </si>
   <si>
     <t>MacOS</t>
-  </si>
-  <si>
-    <t>Redhat</t>
-  </si>
-  <si>
-    <t>Ubuntu</t>
   </si>
   <si>
     <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
@@ -197,18 +191,14 @@
 </t>
   </si>
   <si>
-    <t>## If at ISIS, please test on IDAaaS
-* Either install on a developer mantid IDAaaS instance with credentials [here](https://stfc365.sharepoint.com/:w:/s/isiscomputingdivision-staffsite/ESTnjvxoislDsmpI8vxNyLUBZxw_51y-Qw0OklU_vNgXVA?e=Ih3iLK)
-* Or install via conda on a normal IDAaaS instance:
-  - In terminal, create a new empty environment and activate it
-  - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.</t>
-  </si>
-  <si>
     <t>We must test the installer package and install direct from conda.
 * To install via conda:
   - Use Intel Conda and make sure conda-forge is added to channels
   - In terminal, create a new empty environment and activate it
   - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.</t>
+  </si>
+  <si>
+    <t>Linux</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1115,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1150,7 +1140,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
@@ -1158,24 +1148,20 @@
         <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>28</v>
-      </c>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1218,7 +1204,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2"/>
     </row>
@@ -1242,7 +1228,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4"/>
     </row>
@@ -1254,7 +1240,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5"/>
     </row>
@@ -1266,7 +1252,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6"/>
     </row>
@@ -1278,7 +1264,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7"/>
     </row>

</xml_diff>

<commit_message>
Add files via upload (#109)
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/SmokeTesting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955D629F-D42C-4942-9DFA-F56EDFB02A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FB16BB-06F6-0841-A2A2-2EC1F13FD396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Title</t>
   </si>
@@ -183,22 +183,53 @@
 - [ ] Run through some examples from [the documentation](https://docs.mantidproject.org/nightly/tutorials/python_in_mantid/index.html), 3 or 4 examples from the Solutions is enough </t>
   </si>
   <si>
-    <t xml:space="preserve">* To install the tar.xz package for Linux, run `(sudo) tar -xJf mantid-VA.B.C.tar.xz` in a terminal and it will unzip the package in your current working directory. 
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>* To install the tar.xz package for Linux, run `(sudo) tar -xJf mantid-VA.B.C.tar.xz` in a terminal and it will unzip the package in your current working directory. 
 * To install via conda:
   - Use Intel Conda and make sure conda-forge is added to channels
-  - In terminal, create a new empty environment and activate it
-  - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.
-</t>
-  </si>
-  <si>
-    <t>We must test the installer package and install direct from conda.
+```
+mamba create -n test_mantid_6.6
+mamba activate test_mantid_6.6
+mamba install -c mantid/label/rc1 mantidworkbench --yes
+workbench # to launch
+```</t>
+  </si>
+  <si>
+    <t>We must test both the .dmg installer package and install direct from conda.
 * To install via conda:
   - Use Intel Conda and make sure conda-forge is added to channels
-  - In terminal, create a new empty environment and activate it
-  - run `conda install -c "mantid/label/vA.B.C-rc1" mantidworkbench` , where A.B.C is the release version.</t>
-  </si>
-  <si>
-    <t>Linux</t>
+```
+mamba create -n test_mantid_6.6
+mamba activate test_mantid_6.6
+mamba install -c mantid/label/rc1 mantidworkbench --yes
+workbench # to launch
+```</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We must test both the .exe installer package and install direct from conda.
+* To install via conda:
+  - Use Intel Conda and make sure conda-forge is added to channels
+```
+mamba create -n test_mantid_6.6
+mamba activate test_mantid_6.6
+mamba install -c mantid/label/rc1 mantidworkbench --yes
+workbench </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t># to launch
+```</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -208,7 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +388,14 @@
       <color rgb="FF24292E"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1115,7 +1154,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1140,7 +1179,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
@@ -1148,15 +1187,15 @@
         <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change link to documentation for workspace testing
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mantid-development\documents\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FB16BB-06F6-0841-A2A2-2EC1F13FD396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1656" yWindow="504" windowWidth="25596" windowHeight="15504" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -100,22 +99,6 @@
   </si>
   <si>
     <t>MacOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
-* Show detectors on these workspaces
-* Check Instrument Viewer for these workspaces, follow  documentation for  [Instrument Viewer Widget](https://docs.mantidproject.org/workbench/instrumentviewer.html) and some more detail on the picking tools in the [Basic Course](https://docs.mantidproject.org/tutorials/mantid_basic_course/connecting_data_to_instruments/03_investigating_data.html)
-  - [ ] Render tab 
-  - [ ] Draw tab 
-  - [ ] Pick tab 
-  - [ ] Instrument tree tab 
-* Test 5 - 10 random algorithms, follow [how to run Algorithms](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/algorithms_workspaces_and_histories/02_algorithms.html#algorithms) and [pick your favourite](https://docs.mantidproject.org/algorithms/)
- - [ ] Help button 
- - [ ] Validation of inputs 
- - [ ] Overwriting workspace 
- - [ ] Run the algorithm 
-- [ ] Check right-click options of the workspaces, they are listed [in the documentation](https://www.mantidproject.org/MantidPlot:_The_Workspace_Menu#Save_Nexus).
-</t>
   </si>
   <si>
     <t xml:space="preserve">### Dirty install
@@ -231,11 +214,27 @@
 ```</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
+* Show detectors on these workspaces
+* Check Instrument Viewer for these workspaces, follow  documentation for  [Instrument Viewer Widget](https://docs.mantidproject.org/workbench/instrumentviewer.html) and some more detail on the picking tools in the [Basic Course](https://docs.mantidproject.org/tutorials/mantid_basic_course/connecting_data_to_instruments/03_investigating_data.html)
+  - [ ] Render tab 
+  - [ ] Draw tab 
+  - [ ] Pick tab 
+  - [ ] Instrument tree tab 
+* Test 5 - 10 random algorithms, follow [how to run Algorithms](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/algorithms_workspaces_and_histories/02_algorithms.html#algorithms) and [pick your favourite](https://docs.mantidproject.org/algorithms/)
+ - [ ] Help button 
+ - [ ] Validation of inputs 
+ - [ ] Overwriting workspace 
+ - [ ] Run the algorithm 
+- [ ] Check right-click options of the workspaces, they are listed [in the image in the documentation](https://docs.mantidproject.org/nightly/workbench/workspacetreewidget.html#workbenchworkspacetoolbox).
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -906,23 +905,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -958,23 +940,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1150,20 +1115,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="64.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1174,31 +1139,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
     </row>
@@ -1209,22 +1174,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="46" style="1" customWidth="1"/>
     <col min="3" max="3" width="72.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="20.77734375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1235,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1243,11 +1208,11 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1259,7 +1224,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1267,11 +1232,11 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1279,11 +1244,11 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1291,11 +1256,11 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1303,94 +1268,94 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D20"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D21"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D22"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D23"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D24"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D25"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D26"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D27"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D28"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D29"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D30"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D31"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D32"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G7" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D33" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G7"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D33">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1399,7 +1364,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
update plotting smoke testing template
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mantid-development\documents\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bya67386\work\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60653696-6559-4C0D-81AA-F2DB37499B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1656" yWindow="504" windowWidth="25596" windowHeight="15504" activeTab="1"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -136,26 +137,6 @@
  - [ ] Alter preferences in [File &gt; Settings](https://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/useful/01_save_settings.html#settings) and check they are obeyed</t>
   </si>
   <si>
-    <t>* 1D plotting:[instructions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/loading_and_displaying_data/03_displaying_1D_data.html#displaying-1d-data)
- - [ ] Simple plot 
- - [ ] Another way to plot 
- - [ ] Adding curves to existing plots 
- - [ ] Also, test out [waterfall](https://docs.mantidproject.org/nightly/plotting/WaterfallPlotsHelp.html#waterfall-plots) and [tiled]( https://docs.mantidproject.org/nightly/plotting/1DPlotsHelp.html#tiled-plots)
- - [ ] Check Toolbar buttons
-* 2D plotting: [instructions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/loading_and_displaying_data/04_displaying_2D_data.html#displaying-2d-data)
- - [ ] Plot all spectra 
- - [ ] Change colour map 
- - [ ] [Contour plot](https://docs.mantidproject.org/nightly/plotting/ColorfillPlotsHelp.html#contour-plots) (under 3D menu) 
- - [ ] Check Toolbar buttons
-* [3D plotting](https://docs.mantidproject.org/nightly/plotting/3DPlotsHelp.html):
- - Load some data eg `LOQ7041` from the ISIS sample data
- - [ ] 3D surface
- - [ ] 3D wire frame  
- - [ ] Check Toolbar buttons
- ## Sliceviewer
- - [ ] Overly long instructions (don't spend  long!) and data [here](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html). In particular try editing the data in a workspace while it is open in Sliceviewer!</t>
-  </si>
-  <si>
     <t xml:space="preserve">* Test that the Python scripting window works, [directions here](https://docs.mantidproject.org/nightly/workbench/scriptwindow.html)
  - [ ] Editor options 
  - [ ] Execution options 
@@ -230,11 +211,31 @@
 - [ ] Check right-click options of the workspaces, they are listed [in the image in the documentation](https://docs.mantidproject.org/nightly/workbench/workspacetreewidget.html#workbenchworkspacetoolbox).
 </t>
   </si>
+  <si>
+    <t>* 1D plotting:[instructions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/loading_and_displaying_data/03_displaying_1D_data.html#displaying-1d-data)
+ - [ ] Simple plot 
+ - [ ] Another way to plot 
+ - [ ] Adding curves to existing plots 
+ - [ ] Also, test out [waterfall](https://docs.mantidproject.org/nightly/plotting/WaterfallPlotsHelp.html#waterfall-plots) and [tiled]( https://docs.mantidproject.org/nightly/plotting/1DPlotsHelp.html#tiled-plots)
+ - [ ] Check Toolbar buttons
+* 2D plotting: [instructions](http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/loading_and_displaying_data/04_displaying_2D_data.html#displaying-2d-data)
+ - [ ] Plot all spectra 
+ - [ ] Change colour map 
+ - [ ] [Contour plot](https://docs.mantidproject.org/nightly/plotting/ColorfillPlotsHelp.html#contour-plots) (under 3D menu) 
+ - [ ] Check Toolbar buttons
+* [3D plotting](https://docs.mantidproject.org/nightly/plotting/3DPlotsHelp.html):
+ - Load some data eg `LOQ74041` from the ISIS sample data
+ - [ ] 3D surface
+ - [ ] 3D wire frame  
+ - [ ] Check Toolbar buttons
+ ## Sliceviewer
+ - [ ] Overly long instructions (don't spend  long!) and data [here](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html). In particular try editing the data in a workspace while it is open in Sliceviewer!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -817,7 +818,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="assignees"/>
@@ -830,9 +831,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -870,9 +871,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -907,7 +908,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -942,7 +943,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1115,20 +1116,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="64.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1139,31 +1140,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
     </row>
@@ -1174,22 +1175,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="46" style="1" customWidth="1"/>
-    <col min="3" max="3" width="72.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="72.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1212,7 +1213,7 @@
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1224,7 +1225,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1236,7 +1237,7 @@
       </c>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1244,11 +1245,11 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1256,11 +1257,11 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1268,94 +1269,94 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G7"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D33">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G7" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D33" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1364,7 +1365,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Add IDAaaS to smoke testing template
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bya67386\work\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60653696-6559-4C0D-81AA-F2DB37499B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE42027-970F-49DB-B4A4-C0F56B3B715E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Title</t>
   </si>
@@ -150,52 +150,6 @@
     <t>Linux</t>
   </si>
   <si>
-    <t>* To install the tar.xz package for Linux, run `(sudo) tar -xJf mantid-VA.B.C.tar.xz` in a terminal and it will unzip the package in your current working directory. 
-* To install via conda:
-  - Use Intel Conda and make sure conda-forge is added to channels
-```
-mamba create -n test_mantid_6.6
-mamba activate test_mantid_6.6
-mamba install -c mantid/label/rc1 mantidworkbench --yes
-workbench # to launch
-```</t>
-  </si>
-  <si>
-    <t>We must test both the .dmg installer package and install direct from conda.
-* To install via conda:
-  - Use Intel Conda and make sure conda-forge is added to channels
-```
-mamba create -n test_mantid_6.6
-mamba activate test_mantid_6.6
-mamba install -c mantid/label/rc1 mantidworkbench --yes
-workbench # to launch
-```</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">We must test both the .exe installer package and install direct from conda.
-* To install via conda:
-  - Use Intel Conda and make sure conda-forge is added to channels
-```
-mamba create -n test_mantid_6.6
-mamba activate test_mantid_6.6
-mamba install -c mantid/label/rc1 mantidworkbench --yes
-workbench </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t># to launch
-```</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">* Load some workspaces, try 5 from different instruments
 * Show detectors on these workspaces
 * Check Instrument Viewer for these workspaces, follow  documentation for  [Instrument Viewer Widget](https://docs.mantidproject.org/workbench/instrumentviewer.html) and some more detail on the picking tools in the [Basic Course](https://docs.mantidproject.org/tutorials/mantid_basic_course/connecting_data_to_instruments/03_investigating_data.html)
@@ -230,6 +184,55 @@
  - [ ] Check Toolbar buttons
  ## Sliceviewer
  - [ ] Overly long instructions (don't spend  long!) and data [here](https://developer.mantidproject.org/Testing/SliceViewer/SliceViewer.html). In particular try editing the data in a workspace while it is open in Sliceviewer!</t>
+  </si>
+  <si>
+    <t>IDAaaS</t>
+  </si>
+  <si>
+    <t>An IDAaaS session link will be shared with you. It will either be a no-GPU or a GPU IDAaaS instance. All IDAaaS-installed packages are Conda installs.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We must test both the .exe installer package and install direct from conda.
+* To install via conda:
+  - Use Intel Conda and make sure conda-forge is added to channels
+```
+mamba create -n mantid_rc1 -c mantid/label/v6.8.0rc1 mantidworkbench --yes
+mamba activate mantid_rc1
+workbench </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t># to launch
+```</t>
+    </r>
+  </si>
+  <si>
+    <t>We must test both the .dmg installer package and install direct from conda.
+* To install via conda:
+  - Use Intel Conda and make sure conda-forge is added to channels
+```
+mamba create -n mantid_rc1 -c mantid/label/v6.8.0rc1 mantidworkbench --yes
+mamba activate mantid_rc1
+workbench # to launch
+```</t>
+  </si>
+  <si>
+    <t>* To install the tar.xz package for Linux, run `(sudo) tar -xJf mantid-VA.B.C.tar.xz` in a terminal and it will unzip the package in your current working directory. 
+* To install via conda:
+  - Use Intel Conda and make sure conda-forge is added to channels
+```
+mamba create -n mantid_rc1 -c mantid/label/v6.8.0rc1 mantidworkbench --yes
+mamba activate mantid_rc1
+workbench # to launch
+```</t>
   </si>
 </sst>
 </file>
@@ -1119,17 +1122,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" customWidth="1"/>
+    <col min="2" max="2" width="67.9453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1140,33 +1143,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="173.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="178.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1178,19 +1185,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="2" width="46" style="1" customWidth="1"/>
-    <col min="3" max="3" width="72.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="72.68359375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.68359375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.15625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1213,7 +1220,7 @@
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1225,7 +1232,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1237,7 +1244,7 @@
       </c>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1245,11 +1252,11 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1268,7 @@
       </c>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1269,88 +1276,88 @@
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="16.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D16"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D17"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D18"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D19"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D20"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D21"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D22"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D23"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D24"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D25"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D26"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D27"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D28"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D29"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D30"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D31"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D32"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D33"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update spreadsheets and smoke script
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/SmokeTesting/issue_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-dev\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\documents\Project-Management\Tools\RoadmapUpdate\SmokeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE42027-970F-49DB-B4A4-C0F56B3B715E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5C519B-ED44-43CC-8B96-9157E6826CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1620" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS instructions" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Title</t>
   </si>
@@ -233,6 +233,9 @@
 mamba activate mantid_rc1
 workbench # to launch
 ```</t>
+  </si>
+  <si>
+    <t>MacOS_arm</t>
   </si>
 </sst>
 </file>
@@ -1120,19 +1123,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="67.9453125" customWidth="1"/>
+    <col min="2" max="2" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="173.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" ht="173.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="178.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" ht="178.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
@@ -1167,12 +1170,20 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1186,18 +1197,18 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="46" style="1" customWidth="1"/>
-    <col min="3" max="3" width="72.68359375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.68359375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.15625" style="1"/>
+    <col min="3" max="3" width="72.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1220,7 +1231,7 @@
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1232,7 +1243,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1244,7 +1255,7 @@
       </c>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1256,7 +1267,7 @@
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1268,7 +1279,7 @@
       </c>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1280,84 +1291,84 @@
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D20"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D21"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D22"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D23"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D24"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D25"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D26"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D27"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D28"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D29"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D30"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D31"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D32"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33"/>
     </row>
   </sheetData>

</xml_diff>